<commit_message>
feat: Update schema template and generate JSON schema from Codebook
- Updated multicenter_schema.xlsx in public folder
- Generated rissa_schema.json with 49 columns from Codebook worksheet
- Includes type validation, min/max ranges, allowed values, and date format patterns
</commit_message>
<xml_diff>
--- a/multicenter_schema.xlsx
+++ b/multicenter_schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huangshifeng/Desktop/SSA_multicenter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFF8191-4097-B046-ADB3-59B1433CE4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E2092E-5104-204B-85EC-10A821C9C0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="204">
   <si>
     <t>PNI</t>
   </si>
@@ -255,10 +255,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>方便資料回溯、修正用，交回前必須刪除此欄</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>字串</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -268,30 +264,6 @@
   </si>
   <si>
     <t>各參與中心辨識ID</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft JhengHei"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>缺值</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>允許</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>不允許</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -346,9 +318,6 @@
   <si>
     <t>YYYY-MM-DD</t>
     <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>M / F / Other / Unknown</t>
   </si>
   <si>
     <t>生理性別</t>
@@ -660,20 +629,10 @@
     <t>主要來源（優先）：colonoscopy / sigmoidoscopy 報告的距肛距離（cm）</t>
   </si>
   <si>
-    <t>備援來源：若無內視鏡距離或明顯不可信，才用 MRI（endoscopic correlate / AV distance）</t>
-  </si>
-  <si>
-    <t>若兩者都有：以 colonoscopy 為準（v1.0 先求一致性）</t>
-  </si>
-  <si>
     <t>tumor_height_source</t>
   </si>
   <si>
     <t>tumor_height的來源</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>endo / mri / unknown</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -964,18 +923,11 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>pfannenstiel / midline / trans-anal / stoma_site / other / unknown</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>標本取出位置</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>是否建立保護性造口</t>
-  </si>
-  <si>
-    <t>none / ileostomy / colostomy / unknown</t>
   </si>
   <si>
     <r>
@@ -1023,10 +975,6 @@
   </si>
   <si>
     <t>吻合策略</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>RiSSA / DSA</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -1526,14 +1474,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>complete / nearly complete / incomplete</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>LH / AR / LAR / Other / Unknown</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Tis / 1 / 2 / 3 / 4a / 4b / X</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -1676,23 +1616,7 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>endo</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>LAR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>double J placement</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>midline</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>RiSSA</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -1700,11 +1624,111 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>complete</t>
+    <r>
+      <t xml:space="preserve">0 = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft JhengHei"/>
+        <family val="2"/>
+      </rPr>
+      <t>大腸鏡</t>
+    </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>允許</t>
+    <t>1 = MRI</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>9 = Unknown</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0=Female</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1=Male</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2=Others</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>9=Unknown</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 = LH</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 = AR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 = LAR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">7 = Others </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 = midline</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 =  trans-anal / stoma_site / other / unknown</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 = trans-anal (NOSE)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>3 = stoma_site</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 = None</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 = ileostomy</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 = colostomy</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 = RiSSA</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 = DSA</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 = nearly complete</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 = incomplete</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 = complete</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>方便資料回溯、修正用，交回/上傳前必須刪除此欄</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1879,7 +1903,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1956,9 +1980,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2180,7 +2201,8 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <selection activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="AZ9" sqref="AZ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2258,7 +2280,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>9</v>
@@ -2267,10 +2289,10 @@
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>11</v>
@@ -2336,7 +2358,7 @@
         <v>27</v>
       </c>
       <c r="AJ1" s="3" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="AK1" s="3" t="s">
         <v>26</v>
@@ -2395,16 +2417,16 @@
         <v>42</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="E2" s="23">
         <v>46022</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="G2" s="8">
         <v>78.2</v>
@@ -2424,8 +2446,8 @@
       <c r="L2" s="6">
         <v>18</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>191</v>
+      <c r="M2" s="6">
+        <v>0</v>
       </c>
       <c r="N2" s="6">
         <v>0</v>
@@ -2445,8 +2467,8 @@
       <c r="S2" s="6">
         <v>7</v>
       </c>
-      <c r="T2" s="6" t="s">
-        <v>192</v>
+      <c r="T2" s="6">
+        <v>2</v>
       </c>
       <c r="U2" s="6">
         <v>1</v>
@@ -2455,10 +2477,10 @@
         <v>1</v>
       </c>
       <c r="W2" s="6" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
-      <c r="X2" s="6" t="s">
-        <v>194</v>
+      <c r="X2" s="6">
+        <v>1</v>
       </c>
       <c r="Y2" s="6">
         <v>1</v>
@@ -2466,8 +2488,8 @@
       <c r="Z2" s="6">
         <v>20</v>
       </c>
-      <c r="AA2" s="6" t="s">
-        <v>195</v>
+      <c r="AA2" s="6">
+        <v>0</v>
       </c>
       <c r="AB2" s="6">
         <v>345</v>
@@ -2497,7 +2519,7 @@
         <v>0</v>
       </c>
       <c r="AK2" s="6" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="AL2" s="6">
         <v>0</v>
@@ -2541,8 +2563,8 @@
       <c r="AY2" s="6">
         <v>2</v>
       </c>
-      <c r="AZ2" s="6" t="s">
-        <v>197</v>
+      <c r="AZ2" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:52" ht="16" x14ac:dyDescent="0.2">
@@ -55449,10 +55471,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DF67661-F76D-284C-B9BE-0B444F160A36}">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49:E52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -55460,10 +55482,10 @@
     <col min="1" max="1" width="28.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="117.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="56.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="128.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="128.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>50</v>
       </c>
@@ -55477,13 +55499,10 @@
         <v>53</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
-      <c r="F1" s="20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>4</v>
       </c>
@@ -55491,39 +55510,33 @@
         <v>54</v>
       </c>
       <c r="C2" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>57</v>
+      <c r="E2" s="15" t="s">
+        <v>203</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="15" t="s">
-        <v>61</v>
+      <c r="E3" s="12" t="s">
+        <v>58</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
@@ -55531,967 +55544,972 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="E12" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>60</v>
+    </row>
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>8</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>77</v>
+      <c r="B14" s="12" t="s">
+        <v>78</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
-        <v>6</v>
+      <c r="C14" s="15" t="s">
+        <v>73</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="D14" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>78</v>
+    </row>
+    <row r="15" spans="1:5" ht="38" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
+        <v>165</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>79</v>
+      <c r="B15" s="21" t="s">
+        <v>173</v>
       </c>
-      <c r="E9" s="15" t="s">
-        <v>60</v>
+      <c r="C15" s="12" t="s">
+        <v>99</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="D15" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
-        <v>7</v>
+      <c r="C16" s="15" t="s">
+        <v>71</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="D16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="38" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
-      <c r="D14" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-      <c r="D15" s="12" t="s">
+      <c r="E16" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="F15" s="15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
-      <c r="D16" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
       <c r="D17" s="12" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="E17" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="D18" s="12" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="E18" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
       <c r="D19" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="D20" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="D21" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="D22" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="12"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="12" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="12"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="12" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="14" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
-        <v>10</v>
+      <c r="B27" t="s">
+        <v>98</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="C27" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="F21" t="s">
+      <c r="D27" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="F22" t="s">
+    <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A28" s="14"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
+    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A29" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A30" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A34" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A35" s="14"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="E35" s="15"/>
+    </row>
+    <row r="36" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A36" s="14"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="E36" s="15"/>
+    </row>
+    <row r="37" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A37" s="14"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="E37" s="15"/>
+    </row>
+    <row r="38" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A38" s="14"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="E38" s="15"/>
+    </row>
+    <row r="39" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A39" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A40" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A41" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A42" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A43" s="14"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A44" s="14"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A45" s="14"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A46" s="14"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A47" s="14"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="14"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="14"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A51" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A52" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="E52" s="15"/>
+    </row>
+    <row r="53" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A53" s="14"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E53" s="15"/>
+    </row>
+    <row r="54" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A54" s="14"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="E54" s="15"/>
+    </row>
+    <row r="55" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A55" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E55" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A56" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="E56" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A58" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A60" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A61" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A62" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E62" s="15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A63" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E63" s="17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A64" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="C65" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D65" s="25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B66" s="24"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="25"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67" s="24"/>
+      <c r="C67" s="25"/>
+      <c r="D67" s="25"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B68" s="24"/>
+      <c r="C68" s="25"/>
+      <c r="D68" s="25"/>
+    </row>
+    <row r="69" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A69" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E69" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A70" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B70" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E70" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A71" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D71" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A72" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="E72" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A73" s="14"/>
+      <c r="B73" s="15"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A74" s="14"/>
+      <c r="B74" s="15"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A75" s="14"/>
+      <c r="B75" s="15"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A76" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D76" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A77" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B77" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D77" s="12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A78" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B78" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D78" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A79" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D79" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A80" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B80" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="C80" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A81" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B81" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A82" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="C82" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D82" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="E82" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="15" t="s">
-        <v>103</v>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D83" s="12" t="s">
+        <v>200</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>56</v>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D84" s="12" t="s">
+        <v>202</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A24" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" t="s">
-        <v>106</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A26" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>184</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A28" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A29" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F29" s="17" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A30" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A31" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A32" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A33" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A34" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A35" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A37" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A38" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F38" s="15"/>
-    </row>
-    <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A39" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F39" s="15" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A40" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="E40" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F40" s="15" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A41" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="E41" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A42" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="E42" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A43" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="E43" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A44" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E44" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A45" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A46" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B46" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C46" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="E46" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F46" s="15" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A47" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A48" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F48" s="12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B49" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="C49" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="D49" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="E49" s="26" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B50" s="24"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="26"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B51" s="24"/>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="26"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B52" s="24"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="26"/>
-    </row>
-    <row r="53" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A53" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B53" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E53" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F53" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A54" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="C54" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E54" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F54" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A55" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A56" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="E56" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F56" s="12" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A57" s="14"/>
-      <c r="B57" s="15"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A58" s="14"/>
-      <c r="B58" s="15"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A59" s="14"/>
-      <c r="B59" s="15"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A60" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B60" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="C60" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D60" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="E60" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A61" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B61" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="C61" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="E61" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A62" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E62" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A63" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B63" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="C63" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="D63" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E63" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A64" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B64" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="C64" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E64" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A65" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B65" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="C65" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E65" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A66" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B66" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="C66" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D66" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="E66" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F66" s="15" t="s">
-        <v>110</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="C49:C52"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="E49:E52"/>
+  <mergeCells count="3">
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="C65:C68"/>
+    <mergeCell ref="D65:D68"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>